<commit_message>
Test scripts for Prithwi
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="25">
   <si>
     <t>Emp_id</t>
   </si>
@@ -34,51 +34,61 @@
     <t>message</t>
   </si>
   <si>
-    <t>123456</t>
-  </si>
-  <si>
-    <t>234567</t>
-  </si>
-  <si>
-    <t>test_factorial_case1</t>
-  </si>
-  <si>
-    <t>test_factorial_case2</t>
-  </si>
-  <si>
-    <t>test_factorial_case3</t>
-  </si>
-  <si>
-    <t>test_factorial_case4</t>
-  </si>
-  <si>
-    <t>test_reverse_case1</t>
-  </si>
-  <si>
-    <t>test_reverse_case2</t>
-  </si>
-  <si>
-    <t>test_reverse_case3</t>
-  </si>
-  <si>
-    <t>test_reverse_case4</t>
-  </si>
-  <si>
-    <t>factorial</t>
-  </si>
-  <si>
-    <t>reverse</t>
+    <t>1126673</t>
+  </si>
+  <si>
+    <t>test_factorial_num_case1</t>
+  </si>
+  <si>
+    <t>test_factorial_num_case2</t>
+  </si>
+  <si>
+    <t>test_factorial_num_case3</t>
+  </si>
+  <si>
+    <t>test_factorial_num_case4</t>
+  </si>
+  <si>
+    <t>test_factorial_num_case5</t>
+  </si>
+  <si>
+    <t>test_factorial_num_case6</t>
+  </si>
+  <si>
+    <t>test_even_pos_upcase_case1</t>
+  </si>
+  <si>
+    <t>test_even_pos_upcase_case2</t>
+  </si>
+  <si>
+    <t>test_even_pos_upcase_case3</t>
+  </si>
+  <si>
+    <t>test_even_pos_upcase_case4</t>
+  </si>
+  <si>
+    <t>test_even_pos_upcase_case5</t>
+  </si>
+  <si>
+    <t>test_even_pos_upcase_case6</t>
+  </si>
+  <si>
+    <t>factorial_num</t>
+  </si>
+  <si>
+    <t>even_pos_upcase</t>
+  </si>
+  <si>
+    <t>passed</t>
   </si>
   <si>
     <t>failed</t>
   </si>
   <si>
-    <t>passed</t>
-  </si>
-  <si>
-    <t>assert 1 == 2
-  -1
-  +2</t>
+    <t>TypeError: reduce() of empty sequence with no initial value</t>
+  </si>
+  <si>
+    <t>Failed: DID NOT RAISE &lt;class 'ValueError'&gt;</t>
   </si>
 </sst>
 </file>
@@ -436,7 +446,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -467,19 +477,16 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E2">
-        <v>0.0007195472717285156</v>
-      </c>
-      <c r="F2" t="s">
-        <v>20</v>
+        <v>0.00038909912109375</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -487,16 +494,16 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E3">
-        <v>0.0003552436828613281</v>
+        <v>0.0003588199615478516</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -504,16 +511,16 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E4">
-        <v>0.0003600120544433594</v>
+        <v>0.0003521442413330078</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -521,16 +528,16 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E5">
-        <v>0.0003626346588134766</v>
+        <v>0.0003654956817626953</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -538,16 +545,19 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E6">
-        <v>0.0003991127014160156</v>
+        <v>0.0004706382751464844</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -555,16 +565,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E7">
-        <v>0.0004308223724365233</v>
+        <v>0.0003962516784667969</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -572,16 +585,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E8">
-        <v>0.0003697872161865233</v>
+        <v>0.0003616809844970703</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -589,155 +602,84 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E9">
-        <v>0.0003671646118164063</v>
+        <v>0.0003647804260253906</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E10">
-        <v>0.0006196498870849608</v>
-      </c>
-      <c r="F10" t="s">
-        <v>20</v>
+        <v>0.0004978179931640625</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E11">
-        <v>0.0003767013549804688</v>
+        <v>0.0003888607025146485</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E12">
-        <v>0.000402212142944336</v>
+        <v>0.0004103183746337891</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E13">
-        <v>0.0003621578216552734</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14">
-        <v>0.0003645420074462891</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15">
-        <v>0.0003647804260253906</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16">
-        <v>0.0003573894500732422</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17">
-        <v>0.0003576278686523437</v>
+        <v>0.0003874301910400391</v>
       </c>
     </row>
   </sheetData>

</xml_diff>